<commit_message>
fixed up the Data files.  Converted them to xlsx, and made the data all readable.
</commit_message>
<xml_diff>
--- a/Data/2010_crime.xlsx
+++ b/Data/2010_crime.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Albany</t>
   </si>
@@ -209,6 +209,18 @@
   </si>
   <si>
     <t>New York State</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Violent</t>
+  </si>
+  <si>
+    <t>Property</t>
   </si>
 </sst>
 </file>
@@ -1039,925 +1051,940 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2">
-        <v>3740.3</v>
-      </c>
-      <c r="C1" s="2">
-        <v>402</v>
-      </c>
-      <c r="D1" s="2">
-        <v>3338.3</v>
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>1720.5</v>
+        <v>3740.3</v>
       </c>
       <c r="C2" s="2">
-        <v>183.4</v>
+        <v>402</v>
       </c>
       <c r="D2" s="2">
-        <v>1537.2</v>
+        <v>3338.3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>2450.1999999999998</v>
+        <v>1720.5</v>
       </c>
       <c r="C3" s="2">
-        <v>869.6</v>
+        <v>183.4</v>
       </c>
       <c r="D3" s="2">
-        <v>1580.6</v>
+        <v>1537.2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>3233.6</v>
+        <v>2450.1999999999998</v>
       </c>
       <c r="C4" s="2">
-        <v>260</v>
+        <v>869.6</v>
       </c>
       <c r="D4" s="2">
-        <v>2973.5</v>
+        <v>1580.6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
-        <v>2614.8000000000002</v>
+        <v>3233.6</v>
       </c>
       <c r="C5" s="2">
-        <v>236.3</v>
+        <v>260</v>
       </c>
       <c r="D5" s="2">
-        <v>2378.5</v>
+        <v>2973.5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>2250</v>
+        <v>2614.8000000000002</v>
       </c>
       <c r="C6" s="2">
-        <v>201.5</v>
+        <v>236.3</v>
       </c>
       <c r="D6" s="2">
-        <v>2048.5</v>
+        <v>2378.5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>2939.6</v>
+        <v>2250</v>
       </c>
       <c r="C7" s="2">
-        <v>237.4</v>
+        <v>201.5</v>
       </c>
       <c r="D7" s="2">
-        <v>2702.2</v>
+        <v>2048.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
-        <v>2388.8000000000002</v>
+        <v>2939.6</v>
       </c>
       <c r="C8" s="2">
-        <v>233.1</v>
+        <v>237.4</v>
       </c>
       <c r="D8" s="2">
-        <v>2155.6999999999998</v>
+        <v>2702.2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2">
-        <v>1952.9</v>
+        <v>2388.8000000000002</v>
       </c>
       <c r="C9" s="2">
-        <v>108</v>
+        <v>233.1</v>
       </c>
       <c r="D9" s="2">
-        <v>1844.8</v>
+        <v>2155.6999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2">
-        <v>2261.5</v>
+        <v>1952.9</v>
       </c>
       <c r="C10" s="2">
-        <v>107.6</v>
+        <v>108</v>
       </c>
       <c r="D10" s="2">
-        <v>2154</v>
+        <v>1844.8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2">
-        <v>1865.6</v>
+        <v>2261.5</v>
       </c>
       <c r="C11" s="2">
-        <v>144.80000000000001</v>
+        <v>107.6</v>
       </c>
       <c r="D11" s="2">
-        <v>1720.8</v>
+        <v>2154</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2">
-        <v>2248.9</v>
+        <v>1865.6</v>
       </c>
       <c r="C12" s="2">
-        <v>137.1</v>
+        <v>144.80000000000001</v>
       </c>
       <c r="D12" s="2">
-        <v>2111.8000000000002</v>
+        <v>1720.8</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2">
-        <v>1734.2</v>
+        <v>2248.9</v>
       </c>
       <c r="C13" s="2">
-        <v>138.6</v>
+        <v>137.1</v>
       </c>
       <c r="D13" s="2">
-        <v>1595.6</v>
+        <v>2111.8000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2">
-        <v>1949.6</v>
+        <v>1734.2</v>
       </c>
       <c r="C14" s="2">
-        <v>243.9</v>
+        <v>138.6</v>
       </c>
       <c r="D14" s="2">
-        <v>1705.8</v>
+        <v>1595.6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2">
-        <v>3637.5</v>
+        <v>1949.6</v>
       </c>
       <c r="C15" s="2">
-        <v>505.8</v>
+        <v>243.9</v>
       </c>
       <c r="D15" s="2">
-        <v>3131.6</v>
+        <v>1705.8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2">
-        <v>1454.2</v>
+        <v>3637.5</v>
       </c>
       <c r="C16" s="2">
-        <v>102.9</v>
+        <v>505.8</v>
       </c>
       <c r="D16" s="2">
-        <v>1351.4</v>
+        <v>3131.6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2">
-        <v>1897.9</v>
+        <v>1454.2</v>
       </c>
       <c r="C17" s="2">
-        <v>114.8</v>
+        <v>102.9</v>
       </c>
       <c r="D17" s="2">
-        <v>1783.1</v>
+        <v>1351.4</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" s="2">
-        <v>3108</v>
+        <v>1897.9</v>
       </c>
       <c r="C18" s="2">
-        <v>226.3</v>
+        <v>114.8</v>
       </c>
       <c r="D18" s="2">
-        <v>2881.6</v>
+        <v>1783.1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2">
-        <v>2572.5</v>
+        <v>3108</v>
       </c>
       <c r="C19" s="2">
-        <v>188.1</v>
+        <v>226.3</v>
       </c>
       <c r="D19" s="2">
-        <v>2384.3000000000002</v>
+        <v>2881.6</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2">
-        <v>1691.5</v>
+        <v>2572.5</v>
       </c>
       <c r="C20" s="2">
-        <v>189.8</v>
+        <v>188.1</v>
       </c>
       <c r="D20" s="2">
-        <v>1501.7</v>
+        <v>2384.3000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B21" s="2">
-        <v>1077.9000000000001</v>
+        <v>1691.5</v>
       </c>
       <c r="C21" s="2">
-        <v>82.9</v>
+        <v>189.8</v>
       </c>
       <c r="D21" s="2">
-        <v>995</v>
+        <v>1501.7</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B22" s="2">
-        <v>2209.4</v>
+        <v>1077.9000000000001</v>
       </c>
       <c r="C22" s="2">
-        <v>269</v>
+        <v>82.9</v>
       </c>
       <c r="D22" s="2">
-        <v>1940.3</v>
+        <v>995</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B23" s="2">
-        <v>2052.8000000000002</v>
+        <v>2209.4</v>
       </c>
       <c r="C23" s="2">
-        <v>183.7</v>
+        <v>269</v>
       </c>
       <c r="D23" s="2">
-        <v>1869.1</v>
+        <v>1940.3</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24" s="2">
-        <v>2242</v>
+        <v>2052.8000000000002</v>
       </c>
       <c r="C24" s="2">
-        <v>647.6</v>
+        <v>183.7</v>
       </c>
       <c r="D24" s="2">
-        <v>1594.4</v>
+        <v>1869.1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" s="2">
-        <v>1787.9</v>
+        <v>2242</v>
       </c>
       <c r="C25" s="2">
-        <v>97</v>
+        <v>647.6</v>
       </c>
       <c r="D25" s="2">
-        <v>1690.9</v>
+        <v>1594.4</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26" s="2">
-        <v>1862.3</v>
+        <v>1787.9</v>
       </c>
       <c r="C26" s="2">
-        <v>75.8</v>
+        <v>97</v>
       </c>
       <c r="D26" s="2">
-        <v>1786.5</v>
+        <v>1690.9</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B27" s="2">
-        <v>1763.9</v>
+        <v>1862.3</v>
       </c>
       <c r="C27" s="2">
-        <v>70.8</v>
+        <v>75.8</v>
       </c>
       <c r="D27" s="2">
-        <v>1693.1</v>
+        <v>1786.5</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" s="2">
-        <v>3586.2</v>
+        <v>1763.9</v>
       </c>
       <c r="C28" s="2">
-        <v>389.1</v>
+        <v>70.8</v>
       </c>
       <c r="D28" s="2">
-        <v>3197.1</v>
+        <v>1693.1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="2">
-        <v>2424.5</v>
+        <v>3586.2</v>
       </c>
       <c r="C29" s="2">
-        <v>150.1</v>
+        <v>389.1</v>
       </c>
       <c r="D29" s="2">
-        <v>2274.4</v>
+        <v>3197.1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30" s="2">
-        <v>1510.8</v>
+        <v>2424.5</v>
       </c>
       <c r="C30" s="2">
-        <v>174.2</v>
+        <v>150.1</v>
       </c>
       <c r="D30" s="2">
-        <v>1336.6</v>
+        <v>2274.4</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" s="2">
-        <v>3170</v>
+        <v>1510.8</v>
       </c>
       <c r="C31" s="2">
-        <v>545.6</v>
+        <v>174.2</v>
       </c>
       <c r="D31" s="2">
-        <v>2624.4</v>
+        <v>1336.6</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B32" s="2">
-        <v>3375.4</v>
+        <v>3170</v>
       </c>
       <c r="C32" s="2">
-        <v>392.2</v>
+        <v>545.6</v>
       </c>
       <c r="D32" s="2">
-        <v>2983.2</v>
+        <v>2624.4</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B33" s="2">
-        <v>2726</v>
+        <v>3375.4</v>
       </c>
       <c r="C33" s="2">
-        <v>256.10000000000002</v>
+        <v>392.2</v>
       </c>
       <c r="D33" s="2">
-        <v>2470</v>
+        <v>2983.2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="B34" s="2">
-        <v>2893.1</v>
+        <v>2726</v>
       </c>
       <c r="C34" s="2">
-        <v>357.9</v>
+        <v>256.10000000000002</v>
       </c>
       <c r="D34" s="2">
-        <v>2535.3000000000002</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B35" s="2">
-        <v>1897.9</v>
+        <v>2893.1</v>
       </c>
       <c r="C35" s="2">
-        <v>121.9</v>
+        <v>357.9</v>
       </c>
       <c r="D35" s="2">
-        <v>1776</v>
+        <v>2535.3000000000002</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B36" s="2">
-        <v>2384.5</v>
+        <v>1897.9</v>
       </c>
       <c r="C36" s="2">
-        <v>259.5</v>
+        <v>121.9</v>
       </c>
       <c r="D36" s="2">
-        <v>2125</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B37" s="2">
-        <v>2564.1999999999998</v>
+        <v>2384.5</v>
       </c>
       <c r="C37" s="2">
-        <v>190.9</v>
+        <v>259.5</v>
       </c>
       <c r="D37" s="2">
-        <v>2373.3000000000002</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B38" s="2">
-        <v>2741.3</v>
+        <v>2564.1999999999998</v>
       </c>
       <c r="C38" s="2">
-        <v>157.6</v>
+        <v>190.9</v>
       </c>
       <c r="D38" s="2">
-        <v>2583.6999999999998</v>
+        <v>2373.3000000000002</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B39" s="2">
-        <v>1880</v>
+        <v>2741.3</v>
       </c>
       <c r="C39" s="2">
-        <v>208.5</v>
+        <v>157.6</v>
       </c>
       <c r="D39" s="2">
-        <v>1671.5</v>
+        <v>2583.6999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B40" s="2">
-        <v>947.5</v>
+        <v>1880</v>
       </c>
       <c r="C40" s="2">
-        <v>69.099999999999994</v>
+        <v>208.5</v>
       </c>
       <c r="D40" s="2">
-        <v>878.4</v>
+        <v>1671.5</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B41" s="2">
-        <v>1693.7</v>
+        <v>947.5</v>
       </c>
       <c r="C41" s="2">
-        <v>424.4</v>
+        <v>69.099999999999994</v>
       </c>
       <c r="D41" s="2">
-        <v>1269.3</v>
+        <v>878.4</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B42" s="2">
-        <v>3135.2</v>
+        <v>1693.7</v>
       </c>
       <c r="C42" s="2">
-        <v>354.3</v>
+        <v>424.4</v>
       </c>
       <c r="D42" s="2">
-        <v>2780.9</v>
+        <v>1269.3</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B43" s="2">
-        <v>1396</v>
+        <v>3135.2</v>
       </c>
       <c r="C43" s="2">
-        <v>276.60000000000002</v>
+        <v>354.3</v>
       </c>
       <c r="D43" s="2">
-        <v>1119.4000000000001</v>
+        <v>2780.9</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B44" s="2">
-        <v>1596.8</v>
+        <v>1396</v>
       </c>
       <c r="C44" s="2">
-        <v>154.30000000000001</v>
+        <v>276.60000000000002</v>
       </c>
       <c r="D44" s="2">
-        <v>1442.5</v>
+        <v>1119.4000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B45" s="2">
-        <v>2219.4</v>
+        <v>1596.8</v>
       </c>
       <c r="C45" s="2">
-        <v>127.5</v>
+        <v>154.30000000000001</v>
       </c>
       <c r="D45" s="2">
-        <v>2091.9</v>
+        <v>1442.5</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B46" s="2">
-        <v>1474.1</v>
+        <v>2219.4</v>
       </c>
       <c r="C46" s="2">
-        <v>68.8</v>
+        <v>127.5</v>
       </c>
       <c r="D46" s="2">
-        <v>1405.3</v>
+        <v>2091.9</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B47" s="2">
-        <v>3984.5</v>
+        <v>1474.1</v>
       </c>
       <c r="C47" s="2">
-        <v>494.6</v>
+        <v>68.8</v>
       </c>
       <c r="D47" s="2">
-        <v>3489.9</v>
+        <v>1405.3</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B48" s="2">
-        <v>1498.3</v>
+        <v>3984.5</v>
       </c>
       <c r="C48" s="2">
-        <v>54.5</v>
+        <v>494.6</v>
       </c>
       <c r="D48" s="2">
-        <v>1443.7</v>
+        <v>3489.9</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B49" s="2">
-        <v>1067.5</v>
+        <v>1498.3</v>
       </c>
       <c r="C49" s="2">
-        <v>54.2</v>
+        <v>54.5</v>
       </c>
       <c r="D49" s="2">
-        <v>1013.3</v>
+        <v>1443.7</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B50" s="2">
-        <v>1944.3</v>
+        <v>1067.5</v>
       </c>
       <c r="C50" s="2">
-        <v>154.1</v>
+        <v>54.2</v>
       </c>
       <c r="D50" s="2">
-        <v>1790.2</v>
+        <v>1013.3</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B51" s="2">
-        <v>1928.6</v>
+        <v>1944.3</v>
       </c>
       <c r="C51" s="2">
-        <v>172.2</v>
+        <v>154.1</v>
       </c>
       <c r="D51" s="2">
-        <v>1756.4</v>
+        <v>1790.2</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B52" s="2">
-        <v>2158.6</v>
+        <v>1928.6</v>
       </c>
       <c r="C52" s="2">
-        <v>157.30000000000001</v>
+        <v>172.2</v>
       </c>
       <c r="D52" s="2">
-        <v>2001.3</v>
+        <v>1756.4</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B53" s="2">
-        <v>2270.5</v>
+        <v>2158.6</v>
       </c>
       <c r="C53" s="2">
-        <v>290.10000000000002</v>
+        <v>157.30000000000001</v>
       </c>
       <c r="D53" s="2">
-        <v>1980.4</v>
+        <v>2001.3</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B54" s="2">
-        <v>1135</v>
+        <v>2270.5</v>
       </c>
       <c r="C54" s="2">
-        <v>73</v>
+        <v>290.10000000000002</v>
       </c>
       <c r="D54" s="2">
-        <v>1062</v>
+        <v>1980.4</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B55" s="2">
-        <v>2475.3000000000002</v>
+        <v>1135</v>
       </c>
       <c r="C55" s="2">
-        <v>118.6</v>
+        <v>73</v>
       </c>
       <c r="D55" s="2">
-        <v>2356.6999999999998</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B56" s="2">
-        <v>2135.6</v>
+        <v>2475.3000000000002</v>
       </c>
       <c r="C56" s="2">
-        <v>227</v>
+        <v>118.6</v>
       </c>
       <c r="D56" s="2">
-        <v>1908.6</v>
+        <v>2356.6999999999998</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B57" s="2">
-        <v>1961.9</v>
+        <v>2135.6</v>
       </c>
       <c r="C57" s="2">
-        <v>146.5</v>
+        <v>227</v>
       </c>
       <c r="D57" s="2">
-        <v>1815.4</v>
+        <v>1908.6</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B58" s="2">
-        <v>1412.6</v>
+        <v>1961.9</v>
       </c>
       <c r="C58" s="2">
-        <v>149.5</v>
+        <v>146.5</v>
       </c>
       <c r="D58" s="2">
-        <v>1263.0999999999999</v>
+        <v>1815.4</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B59" s="2">
-        <v>2171.6</v>
+        <v>1412.6</v>
       </c>
       <c r="C59" s="2">
-        <v>186.6</v>
+        <v>149.5</v>
       </c>
       <c r="D59" s="2">
-        <v>1985</v>
+        <v>1263.0999999999999</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B60" s="2">
-        <v>1615.5</v>
+        <v>2171.6</v>
       </c>
       <c r="C60" s="2">
-        <v>258.8</v>
+        <v>186.6</v>
       </c>
       <c r="D60" s="2">
-        <v>1356.7</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B61" s="2">
-        <v>1168.3</v>
+        <v>1615.5</v>
       </c>
       <c r="C61" s="2">
-        <v>81</v>
+        <v>258.8</v>
       </c>
       <c r="D61" s="2">
-        <v>1087.3</v>
+        <v>1356.7</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B62" s="2">
+        <v>1168.3</v>
+      </c>
+      <c r="C62" s="2">
+        <v>81</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1087.3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B63" s="2">
         <v>1960.1</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C63" s="2">
         <v>74.400000000000006</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D63" s="2">
         <v>1885.7</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>60</v>
-      </c>
-      <c r="B64" s="1">
-        <v>2256.5</v>
-      </c>
-      <c r="C64">
-        <v>581.70000000000005</v>
-      </c>
-      <c r="D64" s="1">
-        <v>1674.8</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B65" s="1">
-        <v>2367.5</v>
+        <v>2256.5</v>
       </c>
       <c r="C65">
-        <v>247.3</v>
+        <v>581.70000000000005</v>
       </c>
       <c r="D65" s="1">
-        <v>2120.3000000000002</v>
+        <v>1674.8</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>62</v>
+      </c>
+      <c r="B66" s="1">
+        <v>2367.5</v>
+      </c>
+      <c r="C66">
+        <v>247.3</v>
+      </c>
+      <c r="D66" s="1">
+        <v>2120.3000000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B67" s="1">
         <v>2319.8000000000002</v>
       </c>
-      <c r="C66">
+      <c r="C67">
         <v>391.2</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D67" s="1">
         <v>1928.6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>